<commit_message>
cross-script decoding and new ROIs
</commit_message>
<xml_diff>
--- a/code/stats/experts_vwfa_coordinates.xlsx
+++ b/code/stats/experts_vwfa_coordinates.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cerpelloni/Desktop/GitHub/VisualBraille_data/code/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BC7A29-62FA-6043-88B4-75EEC6AC15EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5101938E-9207-3C43-AC47-D8C139ECD18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -31,6 +31,9 @@
     <t>sub-007</t>
   </si>
   <si>
+    <t>sub-008</t>
+  </si>
+  <si>
     <t>sub-009</t>
   </si>
   <si>
@@ -40,15 +43,15 @@
     <t>sub-013</t>
   </si>
   <si>
-    <t>sub-017</t>
-  </si>
-  <si>
     <t>sub-006</t>
   </si>
   <si>
     <t>sub-007</t>
   </si>
   <si>
+    <t>sub-008</t>
+  </si>
+  <si>
     <t>sub-009</t>
   </si>
   <si>
@@ -56,72 +59,6 @@
   </si>
   <si>
     <t>sub-013</t>
-  </si>
-  <si>
-    <t>sub-017</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>VWFA FR</t>
-  </si>
-  <si>
-    <t>VWFA BR</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>sub-006</t>
-  </si>
-  <si>
-    <t>sub-007</t>
-  </si>
-  <si>
-    <t>sub-008</t>
-  </si>
-  <si>
-    <t>sub-009</t>
-  </si>
-  <si>
-    <t>sub-012</t>
-  </si>
-  <si>
-    <t>sub-013</t>
-  </si>
-  <si>
-    <t>sub-017</t>
-  </si>
-  <si>
-    <t>sub-006</t>
-  </si>
-  <si>
-    <t>sub-007</t>
-  </si>
-  <si>
-    <t>sub-008</t>
-  </si>
-  <si>
-    <t>sub-009</t>
-  </si>
-  <si>
-    <t>sub-012</t>
-  </si>
-  <si>
-    <t>sub-013</t>
-  </si>
-  <si>
-    <t>sub-017</t>
   </si>
   <si>
     <t>Area</t>
@@ -160,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -168,14 +105,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,268 +425,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="true"/>
-    <col min="2" max="2" width="9.28515625" customWidth="true"/>
-    <col min="3" max="3" width="5.42578125" customWidth="true"/>
-    <col min="4" max="4" width="5.42578125" customWidth="true"/>
-    <col min="5" max="5" width="5.42578125" customWidth="true"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="5" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" x14ac:dyDescent="0.2">
-      <c r="A2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="0">
-        <v>-46.799999999999997</v>
-      </c>
-      <c r="D2" s="0">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>-46.8</v>
+      </c>
+      <c r="D2">
         <v>-60</v>
       </c>
-      <c r="E2" s="0">
-        <v>-12.800000000000001</v>
-      </c>
-    </row>
-    <row r="3" x14ac:dyDescent="0.2">
-      <c r="A3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="0">
+      <c r="E2">
+        <v>-12.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
         <v>-52</v>
       </c>
-      <c r="D3" s="0">
-        <v>-49.600000000000001</v>
-      </c>
-      <c r="E3" s="0">
+      <c r="D3">
+        <v>-49.6</v>
+      </c>
+      <c r="E3">
         <v>-18</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.2">
-      <c r="A4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="0">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
         <v>-52</v>
       </c>
-      <c r="D4" s="0">
-        <v>-54.799999999999997</v>
-      </c>
-      <c r="E4" s="0">
+      <c r="D4">
+        <v>-54.8</v>
+      </c>
+      <c r="E4">
         <v>-18</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.2">
-      <c r="A5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="0">
-        <v>-44.200000000000003</v>
-      </c>
-      <c r="D5" s="0">
-        <v>-62.600000000000001</v>
-      </c>
-      <c r="E5" s="0">
-        <v>-12.800000000000001</v>
-      </c>
-    </row>
-    <row r="6" x14ac:dyDescent="0.2">
-      <c r="A6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="0">
-        <v>-44.200000000000003</v>
-      </c>
-      <c r="D6" s="0">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>-44.2</v>
+      </c>
+      <c r="D5">
+        <v>-62.6</v>
+      </c>
+      <c r="E5">
+        <v>-12.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>-44.2</v>
+      </c>
+      <c r="D6">
         <v>-60</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>-15.4</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.2">
-      <c r="A7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="0">
-        <v>-44.200000000000003</v>
-      </c>
-      <c r="D7" s="0">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>-44.2</v>
+      </c>
+      <c r="D7">
         <v>-60</v>
       </c>
-      <c r="E7" s="0">
-        <v>-12.800000000000001</v>
-      </c>
-    </row>
-    <row r="8" x14ac:dyDescent="0.2">
-      <c r="A8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="0">
-        <v>-62.399999999999999</v>
-      </c>
-      <c r="D8" s="0">
-        <v>-47</v>
-      </c>
-      <c r="E8" s="0">
-        <v>-12.800000000000001</v>
-      </c>
-    </row>
-    <row r="9" x14ac:dyDescent="0.2">
-      <c r="A9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="0">
-        <v>-49.399999999999999</v>
-      </c>
-      <c r="D9" s="0">
-        <v>-62.600000000000001</v>
-      </c>
-      <c r="E9" s="0">
-        <v>-12.800000000000001</v>
-      </c>
-    </row>
-    <row r="10" x14ac:dyDescent="0.2">
-      <c r="A10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="0">
+      <c r="E7">
+        <v>-12.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>-49.4</v>
+      </c>
+      <c r="D8">
+        <v>-62.6</v>
+      </c>
+      <c r="E8">
+        <v>-12.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
         <v>-52</v>
       </c>
-      <c r="D10" s="0">
-        <v>-49.600000000000001</v>
-      </c>
-      <c r="E10" s="0">
+      <c r="D9">
+        <v>-49.6</v>
+      </c>
+      <c r="E9">
         <v>-18</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.2">
-      <c r="A11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
-    </row>
-    <row r="12" x14ac:dyDescent="0.2">
-      <c r="A12" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="0">
-        <v>-41.600000000000001</v>
-      </c>
-      <c r="D12" s="0">
-        <v>-62.600000000000001</v>
-      </c>
-      <c r="E12" s="0">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>-41.6</v>
+      </c>
+      <c r="D11">
+        <v>-62.6</v>
+      </c>
+      <c r="E11">
         <v>-10.199999999999999</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.2">
-      <c r="A13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="0">
-        <v>-44.200000000000003</v>
-      </c>
-      <c r="D13" s="0">
-        <v>-57.399999999999999</v>
-      </c>
-      <c r="E13" s="0">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>-44.2</v>
+      </c>
+      <c r="D12">
+        <v>-57.4</v>
+      </c>
+      <c r="E12">
         <v>-18</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="0">
-        <v>-46.799999999999997</v>
-      </c>
-      <c r="D14" s="0">
-        <v>-62.600000000000001</v>
-      </c>
-      <c r="E14" s="0">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>-46.8</v>
+      </c>
+      <c r="D13">
+        <v>-62.6</v>
+      </c>
+      <c r="E13">
         <v>-15.4</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="0">
-        <v>-62.399999999999999</v>
-      </c>
-      <c r="D15" s="0">
-        <v>-47</v>
-      </c>
-      <c r="E15" s="0">
-        <v>-12.800000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>